<commit_message>
Adding the updated code and PLP documents
</commit_message>
<xml_diff>
--- a/Expense_Code/PLP Documents/Review/Code Review/Peer Review/Defect Tracking Sheet/Code_Defect_Tracking.xlsx
+++ b/Expense_Code/PLP Documents/Review/Code Review/Peer Review/Defect Tracking Sheet/Code_Defect_Tracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rjt\PLP\PLP Documents\Review\Code Review\Peer Review\Defect Tracking Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\rvallamb\Desktop\Expense_Code\PLP Documents\Review\Code Review\Peer Review\Defect Tracking Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -658,7 +658,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>Status</t>
   </si>
@@ -804,9 +804,6 @@
     <t>REP</t>
   </si>
   <si>
-    <t xml:space="preserve">PPR </t>
-  </si>
-  <si>
     <t>SR</t>
   </si>
   <si>
@@ -846,71 +843,69 @@
     <t>High</t>
   </si>
   <si>
-    <t>Tanmaya K Acharya</t>
-  </si>
-  <si>
     <t>D_01</t>
   </si>
   <si>
-    <t>D_02</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Eclipse</t>
-  </si>
-  <si>
-    <t>13/03/2017</t>
-  </si>
-  <si>
     <t>Airline Reservation System</t>
   </si>
   <si>
     <t>Group 1</t>
   </si>
   <si>
-    <t>Insert Flight Information Module</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previous date is also accepted. </t>
-  </si>
-  <si>
-    <t>The Departure city and Arrival city must not be same.</t>
-  </si>
-  <si>
-    <t>Ritika Mishra</t>
-  </si>
-  <si>
-    <t>Rajat Bhutani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rajat.aggarwal@capgemini.com
-rabina.chand@capgemini.com
-rajat.bhutani @capgemini.com
-ritika.a.mishra@capgemini.com
-farah.jamal@capgemini.com
-priya.b.kaushik@capgemini.com
-jeeveswar.medavaram@capgemini.com
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>Group 3</t>
+  </si>
+  <si>
+    <t>Expense Management System (Module: Expense Code)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kavya Lekhana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kavya-lekhana.gurramkonda@capgemini.com
+amruta.deokar@capgemini,com
+ranjith.vallambhatla@capgemini.com
+sejal.jain@capgemini.com
+rupesh.vishwakarma@capgemini.com
+karan.upneja@capgemini.com
+manasa.paidi@capgemini.com
+anshu.kumawat@capgemini.com
 </t>
   </si>
   <si>
-    <t>Rajat Aggarwal</t>
-  </si>
-  <si>
-    <t>The Date inserted should be an upcoming date and upto 2 months</t>
-  </si>
-  <si>
-    <t>Depatrure City and Arrival City can be same</t>
-  </si>
-  <si>
-    <t>TC_02</t>
-  </si>
-  <si>
-    <t>ACT</t>
+    <t>Anshu Kumawat</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Update Expense code Module</t>
+  </si>
+  <si>
+    <t>While updation duplicate expense type entry was accepted</t>
+  </si>
+  <si>
+    <t>Expense type against every expense code must be unique. But updation function was allowing the user to update the expense type leading to duplication of expense types in the database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _</t>
+  </si>
+  <si>
+    <t>STS</t>
+  </si>
+  <si>
+    <t>Ranjith Vallambhatla</t>
+  </si>
+  <si>
+    <t>Amruta Deokar</t>
+  </si>
+  <si>
+    <t>Defect detected through Postman</t>
   </si>
 </sst>
 </file>
@@ -1998,7 +1993,7 @@
   <dimension ref="A4:V18"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="17.25" customHeight="1"/>
@@ -2024,7 +2019,7 @@
     </row>
     <row r="6" spans="2:4" ht="17.25" customHeight="1">
       <c r="B6" s="45" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="17.25" customHeight="1">
@@ -2032,7 +2027,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D7" s="48"/>
     </row>
@@ -2041,7 +2036,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" s="48"/>
     </row>
@@ -2063,10 +2058,14 @@
     </row>
     <row r="12" spans="2:4" ht="14.25">
       <c r="B12" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="19"/>
+        <v>68</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="19">
+        <v>43345</v>
+      </c>
     </row>
     <row r="13" spans="2:4" ht="17.25" customHeight="1">
       <c r="B13" s="18" t="s">
@@ -2081,10 +2080,14 @@
     </row>
     <row r="14" spans="2:4" ht="14.25">
       <c r="B14" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="19"/>
+        <v>70</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="19">
+        <v>43345</v>
+      </c>
     </row>
     <row r="15" spans="2:4" ht="17.25" customHeight="1">
       <c r="B15" s="18" t="s">
@@ -2098,9 +2101,7 @@
       </c>
     </row>
     <row r="16" spans="2:4" ht="14.25">
-      <c r="B16" s="42" t="s">
-        <v>62</v>
-      </c>
+      <c r="B16" s="42"/>
       <c r="C16" s="42"/>
       <c r="D16" s="19"/>
     </row>
@@ -2109,7 +2110,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D17" s="21"/>
     </row>
@@ -2117,9 +2118,7 @@
       <c r="B18" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="22">
-        <v>1</v>
-      </c>
+      <c r="C18" s="22"/>
       <c r="D18" s="20"/>
     </row>
   </sheetData>
@@ -2129,12 +2128,15 @@
     <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1" display="kavya-lekhana.gurramkonda@capgemini.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;LTMT/TD05/TMP: January 31, 2011&amp;RClassification: Company Internal&amp;C&amp;"Trebuchet MS,Bold"&amp;10 iGate Public</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2142,8 +2144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2159,7 +2161,8 @@
     <col min="9" max="9" width="9.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="12.28515625" style="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="1"/>
     <col min="16" max="16" width="13" style="1" customWidth="1"/>
@@ -2180,13 +2183,13 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
@@ -2195,12 +2198,12 @@
       <c r="I1" s="49"/>
       <c r="J1" s="11"/>
       <c r="AB1" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:32" customFormat="1" ht="13.5" thickBot="1">
       <c r="AB2" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC2" s="38"/>
       <c r="AD2" s="38"/>
@@ -2284,44 +2287,44 @@
         <v>39</v>
       </c>
       <c r="AB3" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="36" t="s">
         <v>54</v>
-      </c>
-      <c r="AC3" s="36" t="s">
-        <v>55</v>
       </c>
       <c r="AD3" s="36"/>
       <c r="AE3" s="36"/>
       <c r="AF3" s="36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="57.75" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="94.5" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J4" s="8">
         <v>1</v>
@@ -2329,35 +2332,35 @@
       <c r="K4" s="8">
         <v>1</v>
       </c>
-      <c r="L4" s="43" t="s">
-        <v>68</v>
+      <c r="L4" s="43">
+        <v>43345</v>
       </c>
       <c r="M4" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="N4" s="8" t="s">
         <v>77</v>
       </c>
+      <c r="N4" s="43" t="s">
+        <v>77</v>
+      </c>
       <c r="O4" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>48</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="R4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R4" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="S4" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="T4" s="43" t="s">
-        <v>68</v>
+      <c r="S4" s="43">
+        <v>43199</v>
+      </c>
+      <c r="T4" s="43">
+        <v>43199</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="V4" s="8">
         <v>1</v>
@@ -2366,108 +2369,33 @@
         <v>1</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="AA4" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB4" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD4" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE4" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF4" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="AA5" s="38" t="s">
         <v>49</v>
-      </c>
-      <c r="AB4" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC4" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD4" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE4" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF4" s="37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="45">
-      <c r="A5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="8">
-        <v>1</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1</v>
-      </c>
-      <c r="L5" s="43">
-        <v>43042</v>
-      </c>
-      <c r="M5" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="S5" s="43">
-        <v>43042</v>
-      </c>
-      <c r="T5" s="43">
-        <v>43042</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="V5" s="8">
-        <v>1</v>
-      </c>
-      <c r="W5" s="8">
-        <v>1</v>
-      </c>
-      <c r="X5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA5" s="38" t="s">
-        <v>50</v>
       </c>
       <c r="AB5" s="37" t="s">
         <v>47</v>
@@ -2476,7 +2404,7 @@
         <v>45</v>
       </c>
       <c r="AD5" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2485,16 +2413,16 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
       <formula1>defectcategory</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4">
       <formula1>Defectseverity</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4">
       <formula1>defectpriority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P4:P5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P4">
       <formula1>reviewtype</formula1>
     </dataValidation>
   </dataValidations>
@@ -2658,6 +2586,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
@@ -2668,7 +2605,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046351F880B96AE4B9BB4815879ADEBDD" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487f15db4e05f84fdb19aa3f548b93b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81372d4e-bcfc-4844-a57b-a09c5da71958" xmlns:ns3="952a6df7-b138-4f89-9bc4-e7a874ea3254" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09419ac551552483846d59652a820d17" ns2:_="" ns3:_="">
     <xsd:import namespace="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -2838,20 +2775,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B7FC17-EBEF-4DA9-8B6A-7888BA2876BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{257803AA-E8DC-4B99-BE16-A2C66D7E3233}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -2868,7 +2804,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDBF89D9-C125-43F5-92C8-A7A726BA8807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2887,18 +2823,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBFA1F94-87A9-4300-BC74-3C81F405F373}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B7FC17-EBEF-4DA9-8B6A-7888BA2876BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>